<commit_message>
Update radio map by the first trajectory
</commit_message>
<xml_diff>
--- a/RawData/20180307-experiments-records.xlsx
+++ b/RawData/20180307-experiments-records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Wi-Fi参考点" sheetId="1" r:id="rId1"/>
@@ -727,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+    <sheetView topLeftCell="A160" workbookViewId="0">
       <selection activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
@@ -3134,8 +3134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3184,13 +3184,13 @@
         <v>53</v>
       </c>
       <c r="D2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>12</v>
       </c>
       <c r="F2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3199,13 +3199,13 @@
         <v>54</v>
       </c>
       <c r="D3">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3">
         <v>63</v>
       </c>
       <c r="F3">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -3244,13 +3244,13 @@
         <v>66</v>
       </c>
       <c r="D6">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6">
         <v>43</v>
       </c>
       <c r="F6">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3259,13 +3259,13 @@
         <v>58</v>
       </c>
       <c r="D7">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E7">
         <v>65</v>
       </c>
       <c r="F7">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3286,7 +3286,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D9">
         <f>SUM(D2:D8)</f>
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E9">
         <f>SUM(E2:E8)</f>
@@ -3294,7 +3294,7 @@
       </c>
       <c r="F9">
         <f>SUM(F2:F8)</f>
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
wifi sequence distance radiomap finished
</commit_message>
<xml_diff>
--- a/RawData/20180307-experiments-records.xlsx
+++ b/RawData/20180307-experiments-records.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wi-Fi参考点" sheetId="1" r:id="rId1"/>
     <sheet name="抽象地图" sheetId="4" r:id="rId2"/>
     <sheet name="测试轨迹" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="Wi-Fi序列距离_N" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
   <si>
     <t>Num</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -336,6 +336,94 @@
   </si>
   <si>
     <t>QP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试轨迹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机型号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>步数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>起始点x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>起始点y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>终止点x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>终止点y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>360 N5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轨迹描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路径1上并且沿着方向2，并且用作指纹库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-2-test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路径1上并且沿着方向1，并且用作指纹库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路径1上并且沿着方向1，并且用作序列距离测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xiaomi 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-1-test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-1-test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-2-test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路径1上并且沿着方向2，并且用作序列距离测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路径1上并且沿着方向2，并且用作序列距离测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20180508163535_wifi_crowd.csv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -425,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -444,6 +532,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="D181" sqref="D181"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:XFD97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2866,7 +2963,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3134,7 +3231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -3177,7 +3274,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B2" t="s">
@@ -3194,7 +3291,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
+      <c r="A3" s="15"/>
       <c r="B3" t="s">
         <v>54</v>
       </c>
@@ -3209,7 +3306,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>55</v>
       </c>
@@ -3224,7 +3321,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>68</v>
       </c>
@@ -3239,7 +3336,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>66</v>
       </c>
@@ -3254,7 +3351,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>58</v>
       </c>
@@ -3269,7 +3366,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>67</v>
       </c>
@@ -3298,7 +3395,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>59</v>
       </c>
       <c r="B12" t="s">
@@ -3318,7 +3415,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" t="s">
         <v>70</v>
       </c>
@@ -3336,7 +3433,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
+      <c r="A14" s="15"/>
       <c r="B14" t="s">
         <v>71</v>
       </c>
@@ -3379,7 +3476,7 @@
       <c r="A17" s="10"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>61</v>
       </c>
       <c r="B19" t="s">
@@ -3402,7 +3499,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" t="s">
         <v>72</v>
       </c>
@@ -3423,7 +3520,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" t="s">
         <v>73</v>
       </c>
@@ -3444,7 +3541,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" t="s">
         <v>74</v>
       </c>
@@ -3465,7 +3562,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" t="s">
         <v>75</v>
       </c>
@@ -3486,7 +3583,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" t="s">
         <v>76</v>
       </c>
@@ -3507,7 +3604,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" t="s">
         <v>77</v>
       </c>
@@ -3547,13 +3644,340 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="8" max="8" width="34.25" customWidth="1"/>
+    <col min="9" max="9" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2">
+        <v>49.8</v>
+      </c>
+      <c r="E2">
+        <v>10.7</v>
+      </c>
+      <c r="F2">
+        <v>1.2</v>
+      </c>
+      <c r="G2">
+        <v>10.7</v>
+      </c>
+      <c r="H2">
+        <v>63</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3">
+        <v>49.8</v>
+      </c>
+      <c r="E3">
+        <v>10.7</v>
+      </c>
+      <c r="F3">
+        <v>1.2</v>
+      </c>
+      <c r="G3">
+        <v>10.7</v>
+      </c>
+      <c r="H3">
+        <v>63</v>
+      </c>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4">
+        <v>49.8</v>
+      </c>
+      <c r="E4">
+        <v>10.7</v>
+      </c>
+      <c r="F4">
+        <v>1.2</v>
+      </c>
+      <c r="G4">
+        <v>10.7</v>
+      </c>
+      <c r="H4">
+        <v>61</v>
+      </c>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5">
+        <v>1.2</v>
+      </c>
+      <c r="E5">
+        <v>10.7</v>
+      </c>
+      <c r="F5">
+        <v>49.8</v>
+      </c>
+      <c r="G5">
+        <v>10.7</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6">
+        <v>1.2</v>
+      </c>
+      <c r="E6">
+        <v>10.7</v>
+      </c>
+      <c r="F6">
+        <v>49.8</v>
+      </c>
+      <c r="G6">
+        <v>10.7</v>
+      </c>
+      <c r="H6">
+        <v>64</v>
+      </c>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7">
+        <v>1.2</v>
+      </c>
+      <c r="E7">
+        <v>10.7</v>
+      </c>
+      <c r="F7">
+        <v>49.8</v>
+      </c>
+      <c r="G7">
+        <v>10.7</v>
+      </c>
+      <c r="H7">
+        <v>63</v>
+      </c>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="I8" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9">
+        <v>49.8</v>
+      </c>
+      <c r="E9">
+        <v>10.7</v>
+      </c>
+      <c r="F9">
+        <v>1.2</v>
+      </c>
+      <c r="G9">
+        <v>10.7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10">
+        <v>49.8</v>
+      </c>
+      <c r="E10">
+        <v>10.7</v>
+      </c>
+      <c r="F10">
+        <v>1.2</v>
+      </c>
+      <c r="G10">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12">
+        <v>1.2</v>
+      </c>
+      <c r="E12">
+        <v>10.7</v>
+      </c>
+      <c r="F12">
+        <v>49.8</v>
+      </c>
+      <c r="G12">
+        <v>10.7</v>
+      </c>
+      <c r="I12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13">
+        <v>1.2</v>
+      </c>
+      <c r="E13">
+        <v>10.7</v>
+      </c>
+      <c r="F13">
+        <v>49.8</v>
+      </c>
+      <c r="G13">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14">
+        <v>49.8</v>
+      </c>
+      <c r="E14">
+        <v>10.7</v>
+      </c>
+      <c r="F14">
+        <v>1.2</v>
+      </c>
+      <c r="G14">
+        <v>10.7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16">
+        <v>1.2</v>
+      </c>
+      <c r="E16">
+        <v>10.7</v>
+      </c>
+      <c r="F16">
+        <v>49.8</v>
+      </c>
+      <c r="G16">
+        <v>10.7</v>
+      </c>
+      <c r="I16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:A13"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>